<commit_message>
Removed backwards compatibility for multi-sheet bulk app translations
</commit_message>
<xml_diff>
--- a/corehq/apps/translations/tests/data/bulk_app_translation/form_modifications/modifications.xlsx
+++ b/corehq/apps/translations/tests/data/bulk_app_translation/form_modifications/modifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jschweers/Documents/commcare-hq/corehq/apps/app_manager/tests/data/bulk_app_translation/form_modifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B736C9D-6C01-5D40-BE21-ADFECF40F261}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F7142D-7838-E447-B572-32FB0119F011}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Type</t>
   </si>
@@ -36,18 +36,6 @@
   </si>
   <si>
     <t>default_fra</t>
-  </si>
-  <si>
-    <t>icon_filepath_en</t>
-  </si>
-  <si>
-    <t>audio_filepath_en</t>
-  </si>
-  <si>
-    <t>icon_filepath_fra</t>
-  </si>
-  <si>
-    <t>audio_filepath_fra</t>
   </si>
   <si>
     <t>unique_id</t>
@@ -493,7 +481,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -506,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -515,47 +503,47 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -577,10 +565,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -591,24 +579,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -642,49 +630,49 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>